<commit_message>
vision before becoming exe
</commit_message>
<xml_diff>
--- a/meetingtest.xlsx
+++ b/meetingtest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2023c91eea085b67/桌面/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hmttest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{B4D2DADA-BA1B-46A4-874E-A0F7BE3C4707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5EEFB95-B03D-4F57-8873-3C735A8DB3D6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51F21B4-0912-4A2A-B5E7-139551807CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="周工程例会纪要" sheetId="1" r:id="rId1"/>
@@ -188,12 +188,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">
-1.继续推进PR脚本调试及debug
-2.完成内部评测版simd1024代码逻辑综合评估工作</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>1.完成基于beta工程core_l2c模块的布局布线流程
 2.对PR流程及beta工程core_l2c模块相关工作进行总结
 3.在PT环境中查看关键路径时序并尝试优化</t>
@@ -343,6 +337,11 @@
     <t>1.与前端沟通协调全定制SRAM的需求，目前暂定从时序严格和可复用角度将定制器件数量压缩
 2.学习DRC工艺手册，在S14工艺重新更新setup文件后重新跑PR，更换之前用错的lib库
 3.配置S12环境，尝试对corel2c进行布局布线，目前跑到preplace阶段</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.继续推进PR脚本调试及debug
+2.完成内部评测版simd1024代码逻辑综合评估工作</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1333,18 +1332,18 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="5.06640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="39.796875" customWidth="1"/>
-    <col min="5" max="5" width="38.06640625" customWidth="1"/>
+    <col min="4" max="4" width="39.77734375" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="7" max="7" width="37.265625" customWidth="1"/>
-    <col min="8" max="8" width="31.06640625" customWidth="1"/>
+    <col min="7" max="7" width="37.21875" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
     <col min="10" max="31" width="14" customWidth="1"/>
   </cols>
@@ -1461,16 +1460,16 @@
         <v>10</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>8</v>
@@ -1499,7 +1498,7 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31" ht="181.9" customHeight="1">
+    <row r="5" spans="1:31" ht="181.95" customHeight="1">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -1508,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>20</v>
@@ -1561,7 +1560,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>28</v>
@@ -1602,16 +1601,16 @@
         <v>13</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="F7" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="G7" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>49</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>8</v>
@@ -1640,7 +1639,7 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:31" ht="113.75" customHeight="1" thickBot="1">
+    <row r="8" spans="1:31" ht="113.7" customHeight="1" thickBot="1">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -1649,16 +1648,16 @@
         <v>14</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>41</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>42</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>8</v>
@@ -1687,7 +1686,7 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:31" ht="102.4" customHeight="1" thickBot="1">
+    <row r="9" spans="1:31" ht="102.45" customHeight="1" thickBot="1">
       <c r="A9" s="9">
         <v>5</v>
       </c>
@@ -1696,16 +1695,16 @@
         <v>15</v>
       </c>
       <c r="D9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="F9" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>8</v>
@@ -1742,16 +1741,16 @@
         <v>18</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>8</v>
@@ -1788,16 +1787,16 @@
         <v>22</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="F11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="G11" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>8</v>
@@ -7668,6 +7667,6 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>